<commit_message>
v1.1 close the owner status
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_WF_ADMINHOME_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_WF_ADMINHOME_REVIEWS.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8550"/>
   </bookViews>
@@ -10,7 +10,7 @@
     <sheet name="LH_WF-ADMINHOME-REVIEWS-SHEET" sheetId="3" r:id="rId1"/>
     <sheet name="VERSION-HISTORY" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>ID</t>
   </si>
@@ -86,12 +86,15 @@
   </si>
   <si>
     <t>LH_REVIEW_WF_ADMINHOME_001</t>
+  </si>
+  <si>
+    <t>closed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -416,7 +419,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -451,7 +454,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -628,7 +631,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -639,7 +642,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -707,7 +710,7 @@
         <v>19</v>
       </c>
       <c r="H2" s="26" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I2" s="27" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
v1.1 close reviewer varifications
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_WF_ADMINHOME_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_WF_ADMINHOME_REVIEWS.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8550"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7260"/>
   </bookViews>
   <sheets>
     <sheet name="LH_WF-ADMINHOME-REVIEWS-SHEET" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>ID</t>
   </si>
@@ -82,19 +82,22 @@
     <t>Eman Abusalim</t>
   </si>
   <si>
-    <t>open</t>
-  </si>
-  <si>
     <t>LH_REVIEW_WF_ADMINHOME_001</t>
   </si>
   <si>
     <t>closed</t>
+  </si>
+  <si>
+    <t>v1.1</t>
+  </si>
+  <si>
+    <t>close reviewer varifications</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -139,7 +142,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -170,12 +173,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF6F8F9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="8">
     <border>
@@ -284,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -330,15 +327,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -631,7 +619,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -642,7 +630,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -687,33 +675,33 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="28" customFormat="1" ht="75">
-      <c r="A2" s="29" t="s">
+    <row r="2" spans="1:9" s="25" customFormat="1" ht="75">
+      <c r="A2" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="27" t="s">
-        <v>20</v>
+      <c r="I2" s="24" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -844,7 +832,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -884,10 +872,18 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.75">
-      <c r="A3" s="21"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
+      <c r="A3" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="20">
+        <v>45776</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="18.75">
       <c r="A4" s="18"/>

</xml_diff>